<commit_message>
Fix wrong print settings
</commit_message>
<xml_diff>
--- a/hb-back/Tsu.IndividualPlan.WebApi/Storage/SecondPartExample.xlsx
+++ b/hb-back/Tsu.IndividualPlan.WebApi/Storage/SecondPartExample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BathDuck\source\Reposs\tsu-optimize-report\hb-back\Tsu.IndividualPlan.WebApi\Storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ECF036C-489D-490D-8BFC-4B6E49ADC535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61A3FEE6-C5A5-4FB0-81EC-0663A8436142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,6 +23,7 @@
     <sheet name="8_ИРИП ОПВП" sheetId="14" r:id="rId8"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'1_Титульный'!$A$1:$AJ$39</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">'4_УЧ-МЕТ'!$A$1:$F$61</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="4">'5_НДиНМД'!$A$1:$F$61</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="5">'6_НИРС. ОМР '!$A$1:$E$60</definedName>
@@ -2316,69 +2317,69 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="62" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="65" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="66" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="67" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="62" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="62" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="63" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="62" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="62" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="62" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="62" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="63" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="65" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="66" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="67" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="62" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="62" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="62" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="3"/>
     </xf>
@@ -2436,6 +2437,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="3"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2463,17 +2476,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="3"/>
@@ -2500,41 +2531,87 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2548,81 +2625,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="53" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="57" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="55" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="58" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="59" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="59" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2642,24 +2718,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2677,63 +2735,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="59" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="59" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="53" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="55" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="58" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="57" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3097,8 +3098,8 @@
   </sheetPr>
   <dimension ref="A1:AS54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScalePageLayoutView="10" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:AI6"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="10" workbookViewId="0">
+      <selection activeCell="AU22" sqref="AU22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3194,7 +3195,7 @@
       <c r="AS1" s="131"/>
     </row>
     <row r="2" spans="1:45" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="133" t="s">
+      <c r="A2" s="153" t="s">
         <v>306</v>
       </c>
       <c r="B2" s="134"/>
@@ -3243,7 +3244,7 @@
       <c r="AS2" s="131"/>
     </row>
     <row r="3" spans="1:45" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="133" t="s">
+      <c r="A3" s="153" t="s">
         <v>307</v>
       </c>
       <c r="B3" s="134"/>
@@ -3386,7 +3387,7 @@
       <c r="AS5" s="131"/>
     </row>
     <row r="6" spans="1:45" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="135" t="s">
+      <c r="A6" s="154" t="s">
         <v>325</v>
       </c>
       <c r="B6" s="134"/>
@@ -3482,7 +3483,7 @@
       <c r="AS7" s="131"/>
     </row>
     <row r="8" spans="1:45" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="136" t="s">
+      <c r="A8" s="138" t="s">
         <v>307</v>
       </c>
       <c r="B8" s="134"/>
@@ -3531,7 +3532,7 @@
       <c r="AS8" s="131"/>
     </row>
     <row r="9" spans="1:45" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="137" t="s">
+      <c r="A9" s="147" t="s">
         <v>27</v>
       </c>
       <c r="B9" s="134"/>
@@ -3552,7 +3553,7 @@
       <c r="Q9" s="131"/>
       <c r="R9" s="131"/>
       <c r="S9" s="131"/>
-      <c r="T9" s="137" t="s">
+      <c r="T9" s="147" t="s">
         <v>27</v>
       </c>
       <c r="U9" s="134"/>
@@ -3582,7 +3583,7 @@
       <c r="AS9" s="131"/>
     </row>
     <row r="10" spans="1:45" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="137" t="s">
+      <c r="A10" s="147" t="s">
         <v>308</v>
       </c>
       <c r="B10" s="134"/>
@@ -3603,7 +3604,7 @@
       <c r="Q10" s="131"/>
       <c r="R10" s="131"/>
       <c r="S10" s="131"/>
-      <c r="T10" s="137" t="s">
+      <c r="T10" s="147" t="s">
         <v>309</v>
       </c>
       <c r="U10" s="134"/>
@@ -3633,16 +3634,16 @@
       <c r="AS10" s="131"/>
     </row>
     <row r="11" spans="1:45" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="138" t="s">
+      <c r="A11" s="148" t="s">
         <v>307</v>
       </c>
-      <c r="B11" s="138"/>
-      <c r="C11" s="138"/>
-      <c r="D11" s="138"/>
-      <c r="E11" s="138"/>
-      <c r="F11" s="138"/>
-      <c r="G11" s="138"/>
-      <c r="H11" s="138"/>
+      <c r="B11" s="148"/>
+      <c r="C11" s="148"/>
+      <c r="D11" s="148"/>
+      <c r="E11" s="148"/>
+      <c r="F11" s="148"/>
+      <c r="G11" s="148"/>
+      <c r="H11" s="148"/>
       <c r="I11" s="131"/>
       <c r="J11" s="131"/>
       <c r="K11" s="131"/>
@@ -3654,24 +3655,24 @@
       <c r="Q11" s="131"/>
       <c r="R11" s="131"/>
       <c r="S11" s="131"/>
-      <c r="T11" s="138" t="s">
+      <c r="T11" s="148" t="s">
         <v>307</v>
       </c>
-      <c r="U11" s="138"/>
-      <c r="V11" s="138"/>
-      <c r="W11" s="138"/>
-      <c r="X11" s="138"/>
-      <c r="Y11" s="138"/>
-      <c r="Z11" s="138"/>
-      <c r="AA11" s="138"/>
-      <c r="AB11" s="138"/>
-      <c r="AC11" s="138"/>
-      <c r="AD11" s="138"/>
-      <c r="AE11" s="138"/>
-      <c r="AF11" s="138"/>
-      <c r="AG11" s="138"/>
-      <c r="AH11" s="138"/>
-      <c r="AI11" s="138"/>
+      <c r="U11" s="148"/>
+      <c r="V11" s="148"/>
+      <c r="W11" s="148"/>
+      <c r="X11" s="148"/>
+      <c r="Y11" s="148"/>
+      <c r="Z11" s="148"/>
+      <c r="AA11" s="148"/>
+      <c r="AB11" s="148"/>
+      <c r="AC11" s="148"/>
+      <c r="AD11" s="148"/>
+      <c r="AE11" s="148"/>
+      <c r="AF11" s="148"/>
+      <c r="AG11" s="148"/>
+      <c r="AH11" s="148"/>
+      <c r="AI11" s="148"/>
       <c r="AJ11" s="131"/>
       <c r="AK11" s="131"/>
       <c r="AL11" s="131"/>
@@ -3684,7 +3685,7 @@
       <c r="AS11" s="131"/>
     </row>
     <row r="12" spans="1:45" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="139" t="s">
+      <c r="A12" s="149" t="s">
         <v>28</v>
       </c>
       <c r="B12" s="134"/>
@@ -3705,7 +3706,7 @@
       <c r="Q12" s="131"/>
       <c r="R12" s="131"/>
       <c r="S12" s="131"/>
-      <c r="T12" s="139" t="s">
+      <c r="T12" s="149" t="s">
         <v>28</v>
       </c>
       <c r="U12" s="134"/>
@@ -3735,7 +3736,7 @@
       <c r="AS12" s="131"/>
     </row>
     <row r="13" spans="1:45" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="136" t="s">
+      <c r="A13" s="138" t="s">
         <v>307</v>
       </c>
       <c r="B13" s="134"/>
@@ -3784,7 +3785,7 @@
       <c r="AS13" s="131"/>
     </row>
     <row r="14" spans="1:45" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="137" t="s">
+      <c r="A14" s="147" t="s">
         <v>310</v>
       </c>
       <c r="B14" s="134"/>
@@ -3833,16 +3834,16 @@
       <c r="AS14" s="131"/>
     </row>
     <row r="15" spans="1:45" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="138" t="s">
+      <c r="A15" s="148" t="s">
         <v>307</v>
       </c>
-      <c r="B15" s="138"/>
-      <c r="C15" s="138"/>
-      <c r="D15" s="138"/>
-      <c r="E15" s="138"/>
-      <c r="F15" s="138"/>
-      <c r="G15" s="138"/>
-      <c r="H15" s="138"/>
+      <c r="B15" s="148"/>
+      <c r="C15" s="148"/>
+      <c r="D15" s="148"/>
+      <c r="E15" s="148"/>
+      <c r="F15" s="148"/>
+      <c r="G15" s="148"/>
+      <c r="H15" s="148"/>
       <c r="I15" s="131"/>
       <c r="J15" s="131"/>
       <c r="K15" s="131"/>
@@ -3882,7 +3883,7 @@
       <c r="AS15" s="131"/>
     </row>
     <row r="16" spans="1:45" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="139" t="s">
+      <c r="A16" s="149" t="s">
         <v>28</v>
       </c>
       <c r="B16" s="134"/>
@@ -3978,7 +3979,7 @@
       <c r="AS17" s="131"/>
     </row>
     <row r="18" spans="1:45" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="142" t="s">
+      <c r="A18" s="150" t="s">
         <v>311</v>
       </c>
       <c r="B18" s="134"/>
@@ -4027,7 +4028,7 @@
       <c r="AS18" s="131"/>
     </row>
     <row r="19" spans="1:45" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="142" t="s">
+      <c r="A19" s="150" t="s">
         <v>31</v>
       </c>
       <c r="B19" s="134"/>
@@ -4123,7 +4124,7 @@
       <c r="AS20" s="131"/>
     </row>
     <row r="21" spans="1:45" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="136" t="s">
+      <c r="A21" s="138" t="s">
         <v>307</v>
       </c>
       <c r="B21" s="134"/>
@@ -4177,27 +4178,27 @@
       <c r="C22" s="131"/>
       <c r="D22" s="131"/>
       <c r="E22" s="131"/>
-      <c r="F22" s="143" t="s">
+      <c r="F22" s="151" t="s">
         <v>312</v>
       </c>
       <c r="G22" s="134"/>
-      <c r="H22" s="140" t="s">
+      <c r="H22" s="146" t="s">
         <v>313</v>
       </c>
-      <c r="I22" s="140"/>
-      <c r="J22" s="140"/>
-      <c r="K22" s="140"/>
-      <c r="L22" s="144" t="s">
+      <c r="I22" s="146"/>
+      <c r="J22" s="146"/>
+      <c r="K22" s="146"/>
+      <c r="L22" s="152" t="s">
         <v>314</v>
       </c>
       <c r="M22" s="134"/>
       <c r="N22" s="134"/>
-      <c r="O22" s="140" t="s">
+      <c r="O22" s="146" t="s">
         <v>315</v>
       </c>
-      <c r="P22" s="140"/>
-      <c r="Q22" s="140"/>
-      <c r="R22" s="141" t="s">
+      <c r="P22" s="146"/>
+      <c r="Q22" s="146"/>
+      <c r="R22" s="133" t="s">
         <v>316</v>
       </c>
       <c r="S22" s="134"/>
@@ -4229,7 +4230,7 @@
       <c r="AS22" s="131"/>
     </row>
     <row r="23" spans="1:45" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="136" t="s">
+      <c r="A23" s="138" t="s">
         <v>307</v>
       </c>
       <c r="B23" s="134"/>
@@ -4278,7 +4279,7 @@
       <c r="AS23" s="131"/>
     </row>
     <row r="24" spans="1:45" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="145" t="s">
+      <c r="A24" s="144" t="s">
         <v>317</v>
       </c>
       <c r="B24" s="134"/>
@@ -4329,37 +4330,37 @@
     <row r="25" spans="1:45" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="131"/>
       <c r="B25" s="131"/>
-      <c r="C25" s="146" t="s">
+      <c r="C25" s="145" t="s">
         <v>318</v>
       </c>
-      <c r="D25" s="146"/>
-      <c r="E25" s="146"/>
-      <c r="F25" s="146"/>
-      <c r="G25" s="146"/>
-      <c r="H25" s="146"/>
-      <c r="I25" s="146"/>
-      <c r="J25" s="146"/>
-      <c r="K25" s="146"/>
-      <c r="L25" s="146"/>
-      <c r="M25" s="146"/>
-      <c r="N25" s="146"/>
-      <c r="O25" s="146"/>
-      <c r="P25" s="146"/>
-      <c r="Q25" s="146"/>
-      <c r="R25" s="146"/>
-      <c r="S25" s="146"/>
-      <c r="T25" s="146"/>
-      <c r="U25" s="146"/>
-      <c r="V25" s="146"/>
-      <c r="W25" s="146"/>
-      <c r="X25" s="146"/>
-      <c r="Y25" s="146"/>
-      <c r="Z25" s="146"/>
-      <c r="AA25" s="146"/>
-      <c r="AB25" s="146"/>
-      <c r="AC25" s="146"/>
-      <c r="AD25" s="146"/>
-      <c r="AE25" s="146"/>
+      <c r="D25" s="145"/>
+      <c r="E25" s="145"/>
+      <c r="F25" s="145"/>
+      <c r="G25" s="145"/>
+      <c r="H25" s="145"/>
+      <c r="I25" s="145"/>
+      <c r="J25" s="145"/>
+      <c r="K25" s="145"/>
+      <c r="L25" s="145"/>
+      <c r="M25" s="145"/>
+      <c r="N25" s="145"/>
+      <c r="O25" s="145"/>
+      <c r="P25" s="145"/>
+      <c r="Q25" s="145"/>
+      <c r="R25" s="145"/>
+      <c r="S25" s="145"/>
+      <c r="T25" s="145"/>
+      <c r="U25" s="145"/>
+      <c r="V25" s="145"/>
+      <c r="W25" s="145"/>
+      <c r="X25" s="145"/>
+      <c r="Y25" s="145"/>
+      <c r="Z25" s="145"/>
+      <c r="AA25" s="145"/>
+      <c r="AB25" s="145"/>
+      <c r="AC25" s="145"/>
+      <c r="AD25" s="145"/>
+      <c r="AE25" s="145"/>
       <c r="AF25" s="131"/>
       <c r="AG25" s="131"/>
       <c r="AH25" s="131"/>
@@ -4428,39 +4429,39 @@
       <c r="C27" s="132" t="s">
         <v>265</v>
       </c>
-      <c r="D27" s="147" t="s">
+      <c r="D27" s="139" t="s">
         <v>266</v>
       </c>
-      <c r="E27" s="148"/>
-      <c r="F27" s="148"/>
-      <c r="G27" s="148"/>
-      <c r="H27" s="148"/>
-      <c r="I27" s="148"/>
-      <c r="J27" s="148"/>
-      <c r="K27" s="148"/>
-      <c r="L27" s="148"/>
-      <c r="M27" s="148"/>
-      <c r="N27" s="148"/>
-      <c r="O27" s="148"/>
-      <c r="P27" s="148"/>
-      <c r="Q27" s="148"/>
-      <c r="R27" s="148"/>
-      <c r="S27" s="148"/>
-      <c r="T27" s="148"/>
-      <c r="U27" s="148"/>
-      <c r="V27" s="148"/>
-      <c r="W27" s="148"/>
-      <c r="X27" s="148"/>
-      <c r="Y27" s="149"/>
-      <c r="Z27" s="147" t="s">
+      <c r="E27" s="140"/>
+      <c r="F27" s="140"/>
+      <c r="G27" s="140"/>
+      <c r="H27" s="140"/>
+      <c r="I27" s="140"/>
+      <c r="J27" s="140"/>
+      <c r="K27" s="140"/>
+      <c r="L27" s="140"/>
+      <c r="M27" s="140"/>
+      <c r="N27" s="140"/>
+      <c r="O27" s="140"/>
+      <c r="P27" s="140"/>
+      <c r="Q27" s="140"/>
+      <c r="R27" s="140"/>
+      <c r="S27" s="140"/>
+      <c r="T27" s="140"/>
+      <c r="U27" s="140"/>
+      <c r="V27" s="140"/>
+      <c r="W27" s="140"/>
+      <c r="X27" s="140"/>
+      <c r="Y27" s="141"/>
+      <c r="Z27" s="139" t="s">
         <v>287</v>
       </c>
-      <c r="AA27" s="148"/>
-      <c r="AB27" s="148"/>
-      <c r="AC27" s="148"/>
-      <c r="AD27" s="148"/>
-      <c r="AE27" s="148"/>
-      <c r="AF27" s="149"/>
+      <c r="AA27" s="140"/>
+      <c r="AB27" s="140"/>
+      <c r="AC27" s="140"/>
+      <c r="AD27" s="140"/>
+      <c r="AE27" s="140"/>
+      <c r="AF27" s="141"/>
       <c r="AG27" s="131"/>
       <c r="AH27" s="131"/>
       <c r="AI27" s="131"/>
@@ -4481,39 +4482,39 @@
       <c r="C28" s="132" t="s">
         <v>307</v>
       </c>
-      <c r="D28" s="147" t="s">
+      <c r="D28" s="139" t="s">
         <v>307</v>
       </c>
-      <c r="E28" s="148"/>
-      <c r="F28" s="148"/>
-      <c r="G28" s="148"/>
-      <c r="H28" s="148"/>
-      <c r="I28" s="148"/>
-      <c r="J28" s="148"/>
-      <c r="K28" s="148"/>
-      <c r="L28" s="148"/>
-      <c r="M28" s="148"/>
-      <c r="N28" s="148"/>
-      <c r="O28" s="148"/>
-      <c r="P28" s="148"/>
-      <c r="Q28" s="148"/>
-      <c r="R28" s="148"/>
-      <c r="S28" s="148"/>
-      <c r="T28" s="148"/>
-      <c r="U28" s="148"/>
-      <c r="V28" s="148"/>
-      <c r="W28" s="148"/>
-      <c r="X28" s="148"/>
-      <c r="Y28" s="149"/>
-      <c r="Z28" s="147" t="s">
+      <c r="E28" s="140"/>
+      <c r="F28" s="140"/>
+      <c r="G28" s="140"/>
+      <c r="H28" s="140"/>
+      <c r="I28" s="140"/>
+      <c r="J28" s="140"/>
+      <c r="K28" s="140"/>
+      <c r="L28" s="140"/>
+      <c r="M28" s="140"/>
+      <c r="N28" s="140"/>
+      <c r="O28" s="140"/>
+      <c r="P28" s="140"/>
+      <c r="Q28" s="140"/>
+      <c r="R28" s="140"/>
+      <c r="S28" s="140"/>
+      <c r="T28" s="140"/>
+      <c r="U28" s="140"/>
+      <c r="V28" s="140"/>
+      <c r="W28" s="140"/>
+      <c r="X28" s="140"/>
+      <c r="Y28" s="141"/>
+      <c r="Z28" s="139" t="s">
         <v>307</v>
       </c>
-      <c r="AA28" s="148"/>
-      <c r="AB28" s="148"/>
-      <c r="AC28" s="148"/>
-      <c r="AD28" s="148"/>
-      <c r="AE28" s="148"/>
-      <c r="AF28" s="149"/>
+      <c r="AA28" s="140"/>
+      <c r="AB28" s="140"/>
+      <c r="AC28" s="140"/>
+      <c r="AD28" s="140"/>
+      <c r="AE28" s="140"/>
+      <c r="AF28" s="141"/>
       <c r="AG28" s="131"/>
       <c r="AH28" s="131"/>
       <c r="AI28" s="131"/>
@@ -4534,39 +4535,39 @@
       <c r="C29" s="132" t="s">
         <v>307</v>
       </c>
-      <c r="D29" s="147" t="s">
+      <c r="D29" s="139" t="s">
         <v>307</v>
       </c>
-      <c r="E29" s="148"/>
-      <c r="F29" s="148"/>
-      <c r="G29" s="148"/>
-      <c r="H29" s="148"/>
-      <c r="I29" s="148"/>
-      <c r="J29" s="148"/>
-      <c r="K29" s="148"/>
-      <c r="L29" s="148"/>
-      <c r="M29" s="148"/>
-      <c r="N29" s="148"/>
-      <c r="O29" s="148"/>
-      <c r="P29" s="148"/>
-      <c r="Q29" s="148"/>
-      <c r="R29" s="148"/>
-      <c r="S29" s="148"/>
-      <c r="T29" s="148"/>
-      <c r="U29" s="148"/>
-      <c r="V29" s="148"/>
-      <c r="W29" s="148"/>
-      <c r="X29" s="148"/>
-      <c r="Y29" s="149"/>
-      <c r="Z29" s="147" t="s">
+      <c r="E29" s="140"/>
+      <c r="F29" s="140"/>
+      <c r="G29" s="140"/>
+      <c r="H29" s="140"/>
+      <c r="I29" s="140"/>
+      <c r="J29" s="140"/>
+      <c r="K29" s="140"/>
+      <c r="L29" s="140"/>
+      <c r="M29" s="140"/>
+      <c r="N29" s="140"/>
+      <c r="O29" s="140"/>
+      <c r="P29" s="140"/>
+      <c r="Q29" s="140"/>
+      <c r="R29" s="140"/>
+      <c r="S29" s="140"/>
+      <c r="T29" s="140"/>
+      <c r="U29" s="140"/>
+      <c r="V29" s="140"/>
+      <c r="W29" s="140"/>
+      <c r="X29" s="140"/>
+      <c r="Y29" s="141"/>
+      <c r="Z29" s="139" t="s">
         <v>307</v>
       </c>
-      <c r="AA29" s="148"/>
-      <c r="AB29" s="148"/>
-      <c r="AC29" s="148"/>
-      <c r="AD29" s="148"/>
-      <c r="AE29" s="148"/>
-      <c r="AF29" s="149"/>
+      <c r="AA29" s="140"/>
+      <c r="AB29" s="140"/>
+      <c r="AC29" s="140"/>
+      <c r="AD29" s="140"/>
+      <c r="AE29" s="140"/>
+      <c r="AF29" s="141"/>
       <c r="AG29" s="131"/>
       <c r="AH29" s="131"/>
       <c r="AI29" s="131"/>
@@ -4587,39 +4588,39 @@
       <c r="C30" s="132" t="s">
         <v>307</v>
       </c>
-      <c r="D30" s="147" t="s">
+      <c r="D30" s="139" t="s">
         <v>307</v>
       </c>
-      <c r="E30" s="148"/>
-      <c r="F30" s="148"/>
-      <c r="G30" s="148"/>
-      <c r="H30" s="148"/>
-      <c r="I30" s="148"/>
-      <c r="J30" s="148"/>
-      <c r="K30" s="148"/>
-      <c r="L30" s="148"/>
-      <c r="M30" s="148"/>
-      <c r="N30" s="148"/>
-      <c r="O30" s="148"/>
-      <c r="P30" s="148"/>
-      <c r="Q30" s="148"/>
-      <c r="R30" s="148"/>
-      <c r="S30" s="148"/>
-      <c r="T30" s="148"/>
-      <c r="U30" s="148"/>
-      <c r="V30" s="148"/>
-      <c r="W30" s="148"/>
-      <c r="X30" s="148"/>
-      <c r="Y30" s="149"/>
-      <c r="Z30" s="147" t="s">
+      <c r="E30" s="140"/>
+      <c r="F30" s="140"/>
+      <c r="G30" s="140"/>
+      <c r="H30" s="140"/>
+      <c r="I30" s="140"/>
+      <c r="J30" s="140"/>
+      <c r="K30" s="140"/>
+      <c r="L30" s="140"/>
+      <c r="M30" s="140"/>
+      <c r="N30" s="140"/>
+      <c r="O30" s="140"/>
+      <c r="P30" s="140"/>
+      <c r="Q30" s="140"/>
+      <c r="R30" s="140"/>
+      <c r="S30" s="140"/>
+      <c r="T30" s="140"/>
+      <c r="U30" s="140"/>
+      <c r="V30" s="140"/>
+      <c r="W30" s="140"/>
+      <c r="X30" s="140"/>
+      <c r="Y30" s="141"/>
+      <c r="Z30" s="139" t="s">
         <v>307</v>
       </c>
-      <c r="AA30" s="148"/>
-      <c r="AB30" s="148"/>
-      <c r="AC30" s="148"/>
-      <c r="AD30" s="148"/>
-      <c r="AE30" s="148"/>
-      <c r="AF30" s="149"/>
+      <c r="AA30" s="140"/>
+      <c r="AB30" s="140"/>
+      <c r="AC30" s="140"/>
+      <c r="AD30" s="140"/>
+      <c r="AE30" s="140"/>
+      <c r="AF30" s="141"/>
       <c r="AG30" s="131"/>
       <c r="AH30" s="131"/>
       <c r="AI30" s="131"/>
@@ -4682,7 +4683,7 @@
       <c r="AS31" s="131"/>
     </row>
     <row r="32" spans="1:45" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="141" t="s">
+      <c r="A32" s="133" t="s">
         <v>319</v>
       </c>
       <c r="B32" s="134"/>
@@ -4693,16 +4694,16 @@
       <c r="G32" s="134"/>
       <c r="H32" s="134"/>
       <c r="I32" s="134"/>
-      <c r="J32" s="151" t="s">
+      <c r="J32" s="142" t="s">
         <v>320</v>
       </c>
-      <c r="K32" s="151"/>
-      <c r="L32" s="151"/>
-      <c r="M32" s="151"/>
-      <c r="N32" s="151"/>
-      <c r="O32" s="151"/>
-      <c r="P32" s="151"/>
-      <c r="Q32" s="150" t="s">
+      <c r="K32" s="142"/>
+      <c r="L32" s="142"/>
+      <c r="M32" s="142"/>
+      <c r="N32" s="142"/>
+      <c r="O32" s="142"/>
+      <c r="P32" s="142"/>
+      <c r="Q32" s="135" t="s">
         <v>321</v>
       </c>
       <c r="R32" s="134"/>
@@ -4735,7 +4736,7 @@
       <c r="AS32" s="131"/>
     </row>
     <row r="33" spans="1:45" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="141" t="s">
+      <c r="A33" s="133" t="s">
         <v>322</v>
       </c>
       <c r="B33" s="134"/>
@@ -4746,16 +4747,16 @@
       <c r="G33" s="134"/>
       <c r="H33" s="134"/>
       <c r="I33" s="134"/>
-      <c r="J33" s="152" t="s">
+      <c r="J33" s="143" t="s">
         <v>307</v>
       </c>
-      <c r="K33" s="152"/>
-      <c r="L33" s="152"/>
-      <c r="M33" s="152"/>
-      <c r="N33" s="152"/>
-      <c r="O33" s="152"/>
-      <c r="P33" s="152"/>
-      <c r="Q33" s="150" t="s">
+      <c r="K33" s="143"/>
+      <c r="L33" s="143"/>
+      <c r="M33" s="143"/>
+      <c r="N33" s="143"/>
+      <c r="O33" s="143"/>
+      <c r="P33" s="143"/>
+      <c r="Q33" s="135" t="s">
         <v>321</v>
       </c>
       <c r="R33" s="134"/>
@@ -4797,7 +4798,7 @@
       <c r="G34" s="131"/>
       <c r="H34" s="131"/>
       <c r="I34" s="131"/>
-      <c r="J34" s="141" t="s">
+      <c r="J34" s="133" t="s">
         <v>323</v>
       </c>
       <c r="K34" s="134"/>
@@ -4811,7 +4812,7 @@
       <c r="S34" s="131"/>
       <c r="T34" s="131"/>
       <c r="U34" s="131"/>
-      <c r="V34" s="150" t="s">
+      <c r="V34" s="135" t="s">
         <v>30</v>
       </c>
       <c r="W34" s="134"/>
@@ -4855,13 +4856,13 @@
       <c r="N35" s="134"/>
       <c r="O35" s="134"/>
       <c r="P35" s="134"/>
-      <c r="Q35" s="153" t="s">
+      <c r="Q35" s="136" t="s">
         <v>307</v>
       </c>
-      <c r="R35" s="153"/>
-      <c r="S35" s="153"/>
-      <c r="T35" s="153"/>
-      <c r="U35" s="153"/>
+      <c r="R35" s="136"/>
+      <c r="S35" s="136"/>
+      <c r="T35" s="136"/>
+      <c r="U35" s="136"/>
       <c r="V35" s="134"/>
       <c r="W35" s="134"/>
       <c r="X35" s="134"/>
@@ -4904,11 +4905,11 @@
       <c r="N36" s="131"/>
       <c r="O36" s="131"/>
       <c r="P36" s="131"/>
-      <c r="Q36" s="154"/>
-      <c r="R36" s="154"/>
-      <c r="S36" s="154"/>
-      <c r="T36" s="154"/>
-      <c r="U36" s="154"/>
+      <c r="Q36" s="137"/>
+      <c r="R36" s="137"/>
+      <c r="S36" s="137"/>
+      <c r="T36" s="137"/>
+      <c r="U36" s="137"/>
       <c r="V36" s="131"/>
       <c r="W36" s="131"/>
       <c r="X36" s="131"/>
@@ -4982,7 +4983,7 @@
       <c r="AS37" s="131"/>
     </row>
     <row r="38" spans="1:45" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="150" t="s">
+      <c r="A38" s="135" t="s">
         <v>324</v>
       </c>
       <c r="B38" s="134"/>
@@ -5078,7 +5079,7 @@
       <c r="AS39" s="131"/>
     </row>
     <row r="40" spans="1:45" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="136" t="s">
+      <c r="A40" s="138" t="s">
         <v>307</v>
       </c>
       <c r="B40" s="134"/>
@@ -5134,11 +5135,35 @@
     <row r="54" s="130" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="J34:P35"/>
-    <mergeCell ref="V34:AB35"/>
-    <mergeCell ref="Q35:U36"/>
-    <mergeCell ref="A38:AI38"/>
-    <mergeCell ref="A40:AI40"/>
+    <mergeCell ref="A2:AI2"/>
+    <mergeCell ref="A3:AI3"/>
+    <mergeCell ref="A6:AI6"/>
+    <mergeCell ref="A8:AI8"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="T9:AI9"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="T10:AI10"/>
+    <mergeCell ref="A11:H11"/>
+    <mergeCell ref="T11:AI11"/>
+    <mergeCell ref="A12:H12"/>
+    <mergeCell ref="T12:AI12"/>
+    <mergeCell ref="O22:Q22"/>
+    <mergeCell ref="R22:V22"/>
+    <mergeCell ref="A13:AI13"/>
+    <mergeCell ref="A14:AE14"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="A16:H16"/>
+    <mergeCell ref="A18:AI18"/>
+    <mergeCell ref="A19:AI19"/>
+    <mergeCell ref="A21:AI21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="H22:K22"/>
+    <mergeCell ref="L22:N22"/>
+    <mergeCell ref="A23:AI23"/>
+    <mergeCell ref="A24:AI24"/>
+    <mergeCell ref="C25:AE25"/>
+    <mergeCell ref="D27:Y27"/>
+    <mergeCell ref="Z27:AF27"/>
     <mergeCell ref="Q33:U33"/>
     <mergeCell ref="D28:Y28"/>
     <mergeCell ref="Z28:AF28"/>
@@ -5151,38 +5176,14 @@
     <mergeCell ref="Q32:U32"/>
     <mergeCell ref="A33:I33"/>
     <mergeCell ref="J33:P33"/>
-    <mergeCell ref="A23:AI23"/>
-    <mergeCell ref="A24:AI24"/>
-    <mergeCell ref="C25:AE25"/>
-    <mergeCell ref="D27:Y27"/>
-    <mergeCell ref="Z27:AF27"/>
-    <mergeCell ref="O22:Q22"/>
-    <mergeCell ref="R22:V22"/>
-    <mergeCell ref="A13:AI13"/>
-    <mergeCell ref="A14:AE14"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="A16:H16"/>
-    <mergeCell ref="A18:AI18"/>
-    <mergeCell ref="A19:AI19"/>
-    <mergeCell ref="A21:AI21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="H22:K22"/>
-    <mergeCell ref="L22:N22"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="T10:AI10"/>
-    <mergeCell ref="A11:H11"/>
-    <mergeCell ref="T11:AI11"/>
-    <mergeCell ref="A12:H12"/>
-    <mergeCell ref="T12:AI12"/>
-    <mergeCell ref="A2:AI2"/>
-    <mergeCell ref="A3:AI3"/>
-    <mergeCell ref="A6:AI6"/>
-    <mergeCell ref="A8:AI8"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="T9:AI9"/>
+    <mergeCell ref="J34:P35"/>
+    <mergeCell ref="V34:AB35"/>
+    <mergeCell ref="Q35:U36"/>
+    <mergeCell ref="A38:AI38"/>
+    <mergeCell ref="A40:AI40"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="9" pageOrder="overThenDown" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" pageOrder="overThenDown" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6968,14 +6969,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="174" t="s">
+      <c r="A1" s="178" t="s">
         <v>305</v>
       </c>
-      <c r="B1" s="174"/>
-      <c r="C1" s="174"/>
-      <c r="D1" s="174"/>
-      <c r="E1" s="174"/>
-      <c r="F1" s="174"/>
+      <c r="B1" s="178"/>
+      <c r="C1" s="178"/>
+      <c r="D1" s="178"/>
+      <c r="E1" s="178"/>
+      <c r="F1" s="178"/>
       <c r="H1" s="61"/>
       <c r="I1" s="35"/>
       <c r="J1" s="36"/>
@@ -6986,33 +6987,33 @@
       <c r="O1" s="62"/>
     </row>
     <row r="2" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="175" t="s">
+      <c r="A2" s="179" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="175"/>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
-      <c r="E2" s="175"/>
-      <c r="F2" s="175"/>
+      <c r="B2" s="179"/>
+      <c r="C2" s="179"/>
+      <c r="D2" s="179"/>
+      <c r="E2" s="179"/>
+      <c r="F2" s="179"/>
     </row>
     <row r="3" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="181" t="s">
+      <c r="A3" s="185" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="172" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="172"/>
-      <c r="D3" s="186" t="s">
+      <c r="D3" s="177" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="186"/>
-      <c r="F3" s="179" t="s">
+      <c r="E3" s="177"/>
+      <c r="F3" s="183" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="182"/>
+      <c r="A4" s="186"/>
       <c r="B4" s="70" t="s">
         <v>6</v>
       </c>
@@ -7025,17 +7026,17 @@
       <c r="E4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="180"/>
+      <c r="F4" s="184"/>
     </row>
     <row r="5" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="176" t="s">
+      <c r="A5" s="180" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="177"/>
-      <c r="C5" s="177"/>
-      <c r="D5" s="177"/>
-      <c r="E5" s="177"/>
-      <c r="F5" s="178"/>
+      <c r="B5" s="181"/>
+      <c r="C5" s="181"/>
+      <c r="D5" s="181"/>
+      <c r="E5" s="181"/>
+      <c r="F5" s="182"/>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
@@ -7473,14 +7474,14 @@
       <c r="N32" s="98"/>
     </row>
     <row r="33" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="183" t="s">
+      <c r="A33" s="174" t="s">
         <v>8</v>
       </c>
-      <c r="B33" s="184"/>
-      <c r="C33" s="184"/>
-      <c r="D33" s="184"/>
-      <c r="E33" s="184"/>
-      <c r="F33" s="185"/>
+      <c r="B33" s="175"/>
+      <c r="C33" s="175"/>
+      <c r="D33" s="175"/>
+      <c r="E33" s="175"/>
+      <c r="F33" s="176"/>
       <c r="G33" s="116"/>
       <c r="H33" s="99"/>
       <c r="I33" s="98"/>
@@ -8318,17 +8319,17 @@
     <sortCondition ref="A100"/>
   </sortState>
   <mergeCells count="11">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="A3:A4"/>
     <mergeCell ref="A60:C60"/>
     <mergeCell ref="A61:C61"/>
     <mergeCell ref="A33:F33"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="A32:C32"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="A3:A4"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="I1">
@@ -8367,13 +8368,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="202" t="s">
+      <c r="A1" s="189" t="s">
         <v>260</v>
       </c>
-      <c r="B1" s="202"/>
-      <c r="C1" s="202"/>
-      <c r="D1" s="202"/>
-      <c r="E1" s="202"/>
+      <c r="B1" s="189"/>
+      <c r="C1" s="189"/>
+      <c r="D1" s="189"/>
+      <c r="E1" s="189"/>
       <c r="G1" s="61"/>
       <c r="H1" s="35"/>
       <c r="I1" s="34"/>
@@ -8383,27 +8384,27 @@
       <c r="A2" s="169" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="190" t="s">
+      <c r="B2" s="200" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="208" t="s">
+      <c r="C2" s="195" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="208"/>
-      <c r="E2" s="206" t="s">
+      <c r="D2" s="195"/>
+      <c r="E2" s="193" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="189"/>
-      <c r="B3" s="191"/>
+      <c r="A3" s="199"/>
+      <c r="B3" s="201"/>
       <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="207"/>
+      <c r="E3" s="194"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="118"/>
@@ -8705,28 +8706,28 @@
       <c r="I30" s="98"/>
     </row>
     <row r="31" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="209" t="s">
+      <c r="A31" s="196" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="209"/>
-      <c r="C31" s="209"/>
-      <c r="D31" s="209"/>
-      <c r="E31" s="209"/>
+      <c r="B31" s="196"/>
+      <c r="C31" s="196"/>
+      <c r="D31" s="196"/>
+      <c r="E31" s="196"/>
       <c r="F31" s="98"/>
       <c r="G31" s="99"/>
       <c r="H31" s="98"/>
       <c r="I31" s="98"/>
     </row>
     <row r="32" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="192" t="s">
+      <c r="A32" s="202" t="s">
         <v>19</v>
       </c>
-      <c r="B32" s="193"/>
-      <c r="C32" s="203" t="s">
+      <c r="B32" s="203"/>
+      <c r="C32" s="190" t="s">
         <v>15</v>
       </c>
-      <c r="D32" s="203"/>
-      <c r="E32" s="204" t="s">
+      <c r="D32" s="190"/>
+      <c r="E32" s="191" t="s">
         <v>16</v>
       </c>
       <c r="F32" s="98"/>
@@ -8735,23 +8736,23 @@
       <c r="I32" s="98"/>
     </row>
     <row r="33" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="194"/>
-      <c r="B33" s="195"/>
+      <c r="A33" s="204"/>
+      <c r="B33" s="205"/>
       <c r="C33" s="40" t="s">
         <v>4</v>
       </c>
       <c r="D33" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="E33" s="205"/>
+      <c r="E33" s="192"/>
       <c r="F33" s="98"/>
       <c r="G33" s="99"/>
       <c r="H33" s="98"/>
       <c r="I33" s="98"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="196"/>
-      <c r="B34" s="197"/>
+      <c r="A34" s="206"/>
+      <c r="B34" s="207"/>
       <c r="C34" s="50"/>
       <c r="D34" s="51"/>
       <c r="E34" s="52"/>
@@ -8761,8 +8762,8 @@
       <c r="I34" s="98"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="198"/>
-      <c r="B35" s="199"/>
+      <c r="A35" s="187"/>
+      <c r="B35" s="188"/>
       <c r="C35" s="53"/>
       <c r="D35" s="54"/>
       <c r="E35" s="55"/>
@@ -8772,8 +8773,8 @@
       <c r="I35" s="98"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" s="198"/>
-      <c r="B36" s="199"/>
+      <c r="A36" s="187"/>
+      <c r="B36" s="188"/>
       <c r="C36" s="50"/>
       <c r="D36" s="51"/>
       <c r="E36" s="52"/>
@@ -8783,8 +8784,8 @@
       <c r="I36" s="98"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="198"/>
-      <c r="B37" s="199"/>
+      <c r="A37" s="187"/>
+      <c r="B37" s="188"/>
       <c r="C37" s="53"/>
       <c r="D37" s="54"/>
       <c r="E37" s="55"/>
@@ -8794,8 +8795,8 @@
       <c r="I37" s="98"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" s="198"/>
-      <c r="B38" s="199"/>
+      <c r="A38" s="187"/>
+      <c r="B38" s="188"/>
       <c r="C38" s="50"/>
       <c r="D38" s="51"/>
       <c r="E38" s="52"/>
@@ -8805,8 +8806,8 @@
       <c r="I38" s="98"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39" s="198"/>
-      <c r="B39" s="199"/>
+      <c r="A39" s="187"/>
+      <c r="B39" s="188"/>
       <c r="C39" s="53"/>
       <c r="D39" s="54"/>
       <c r="E39" s="55"/>
@@ -8816,8 +8817,8 @@
       <c r="I39" s="98"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40" s="198"/>
-      <c r="B40" s="199"/>
+      <c r="A40" s="187"/>
+      <c r="B40" s="188"/>
       <c r="C40" s="50"/>
       <c r="D40" s="51"/>
       <c r="E40" s="52"/>
@@ -8827,8 +8828,8 @@
       <c r="I40" s="98"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" s="198"/>
-      <c r="B41" s="199"/>
+      <c r="A41" s="187"/>
+      <c r="B41" s="188"/>
       <c r="C41" s="53"/>
       <c r="D41" s="54"/>
       <c r="E41" s="55"/>
@@ -8838,8 +8839,8 @@
       <c r="I41" s="98"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42" s="198"/>
-      <c r="B42" s="199"/>
+      <c r="A42" s="187"/>
+      <c r="B42" s="188"/>
       <c r="C42" s="50"/>
       <c r="D42" s="51"/>
       <c r="E42" s="52"/>
@@ -8849,8 +8850,8 @@
       <c r="I42" s="98"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" s="198"/>
-      <c r="B43" s="199"/>
+      <c r="A43" s="187"/>
+      <c r="B43" s="188"/>
       <c r="C43" s="53"/>
       <c r="D43" s="54"/>
       <c r="E43" s="55"/>
@@ -8860,8 +8861,8 @@
       <c r="I43" s="98"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" s="198"/>
-      <c r="B44" s="199"/>
+      <c r="A44" s="187"/>
+      <c r="B44" s="188"/>
       <c r="C44" s="50"/>
       <c r="D44" s="51"/>
       <c r="E44" s="52"/>
@@ -8871,8 +8872,8 @@
       <c r="I44" s="98"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A45" s="198"/>
-      <c r="B45" s="199"/>
+      <c r="A45" s="187"/>
+      <c r="B45" s="188"/>
       <c r="C45" s="53"/>
       <c r="D45" s="54"/>
       <c r="E45" s="55"/>
@@ -8882,8 +8883,8 @@
       <c r="I45" s="98"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A46" s="198"/>
-      <c r="B46" s="199"/>
+      <c r="A46" s="187"/>
+      <c r="B46" s="188"/>
       <c r="C46" s="50"/>
       <c r="D46" s="51"/>
       <c r="E46" s="52"/>
@@ -8893,8 +8894,8 @@
       <c r="I46" s="98"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A47" s="198"/>
-      <c r="B47" s="199"/>
+      <c r="A47" s="187"/>
+      <c r="B47" s="188"/>
       <c r="C47" s="53"/>
       <c r="D47" s="54"/>
       <c r="E47" s="55"/>
@@ -8904,8 +8905,8 @@
       <c r="I47" s="98"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" s="198"/>
-      <c r="B48" s="199"/>
+      <c r="A48" s="187"/>
+      <c r="B48" s="188"/>
       <c r="C48" s="50"/>
       <c r="D48" s="51"/>
       <c r="E48" s="52"/>
@@ -8915,8 +8916,8 @@
       <c r="I48" s="98"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A49" s="198"/>
-      <c r="B49" s="199"/>
+      <c r="A49" s="187"/>
+      <c r="B49" s="188"/>
       <c r="C49" s="53"/>
       <c r="D49" s="54"/>
       <c r="E49" s="55"/>
@@ -8926,8 +8927,8 @@
       <c r="I49" s="98"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A50" s="198"/>
-      <c r="B50" s="199"/>
+      <c r="A50" s="187"/>
+      <c r="B50" s="188"/>
       <c r="C50" s="50"/>
       <c r="D50" s="51"/>
       <c r="E50" s="52"/>
@@ -8937,8 +8938,8 @@
       <c r="I50" s="98"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A51" s="198"/>
-      <c r="B51" s="199"/>
+      <c r="A51" s="187"/>
+      <c r="B51" s="188"/>
       <c r="C51" s="53"/>
       <c r="D51" s="54"/>
       <c r="E51" s="55"/>
@@ -8948,8 +8949,8 @@
       <c r="I51" s="98"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A52" s="198"/>
-      <c r="B52" s="199"/>
+      <c r="A52" s="187"/>
+      <c r="B52" s="188"/>
       <c r="C52" s="50"/>
       <c r="D52" s="51"/>
       <c r="E52" s="52"/>
@@ -8959,8 +8960,8 @@
       <c r="I52" s="98"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A53" s="198"/>
-      <c r="B53" s="199"/>
+      <c r="A53" s="187"/>
+      <c r="B53" s="188"/>
       <c r="C53" s="53"/>
       <c r="D53" s="54"/>
       <c r="E53" s="55"/>
@@ -8970,8 +8971,8 @@
       <c r="I53" s="98"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A54" s="198"/>
-      <c r="B54" s="199"/>
+      <c r="A54" s="187"/>
+      <c r="B54" s="188"/>
       <c r="C54" s="50"/>
       <c r="D54" s="51"/>
       <c r="E54" s="52"/>
@@ -8981,8 +8982,8 @@
       <c r="I54" s="98"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A55" s="198"/>
-      <c r="B55" s="199"/>
+      <c r="A55" s="187"/>
+      <c r="B55" s="188"/>
       <c r="C55" s="53"/>
       <c r="D55" s="54"/>
       <c r="E55" s="55"/>
@@ -8992,8 +8993,8 @@
       <c r="I55" s="98"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A56" s="198"/>
-      <c r="B56" s="199"/>
+      <c r="A56" s="187"/>
+      <c r="B56" s="188"/>
       <c r="C56" s="50"/>
       <c r="D56" s="51"/>
       <c r="E56" s="52"/>
@@ -9003,8 +9004,8 @@
       <c r="I56" s="98"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A57" s="198"/>
-      <c r="B57" s="199"/>
+      <c r="A57" s="187"/>
+      <c r="B57" s="188"/>
       <c r="C57" s="53"/>
       <c r="D57" s="54"/>
       <c r="E57" s="55"/>
@@ -9014,8 +9015,8 @@
       <c r="I57" s="98"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A58" s="198"/>
-      <c r="B58" s="199"/>
+      <c r="A58" s="187"/>
+      <c r="B58" s="188"/>
       <c r="C58" s="50"/>
       <c r="D58" s="51"/>
       <c r="E58" s="52"/>
@@ -9025,8 +9026,8 @@
       <c r="I58" s="98"/>
     </row>
     <row r="59" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="200"/>
-      <c r="B59" s="201"/>
+      <c r="A59" s="208"/>
+      <c r="B59" s="209"/>
       <c r="C59" s="40"/>
       <c r="D59" s="56"/>
       <c r="E59" s="57"/>
@@ -9036,10 +9037,10 @@
       <c r="I59" s="98"/>
     </row>
     <row r="60" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="187" t="s">
+      <c r="A60" s="197" t="s">
         <v>17</v>
       </c>
-      <c r="B60" s="188"/>
+      <c r="B60" s="198"/>
       <c r="C60" s="107"/>
       <c r="D60" s="108"/>
       <c r="E60" s="109"/>
@@ -9454,27 +9455,6 @@
     <sortCondition ref="A110"/>
   </sortState>
   <mergeCells count="37">
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A31:E31"/>
     <mergeCell ref="A60:B60"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
@@ -9491,6 +9471,27 @@
     <mergeCell ref="A48:B48"/>
     <mergeCell ref="A50:B50"/>
     <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A31:E31"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A41:B41"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="H1">
@@ -9529,13 +9530,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="202" t="s">
+      <c r="A1" s="189" t="s">
         <v>261</v>
       </c>
-      <c r="B1" s="202"/>
-      <c r="C1" s="202"/>
-      <c r="D1" s="202"/>
-      <c r="E1" s="202"/>
+      <c r="B1" s="189"/>
+      <c r="C1" s="189"/>
+      <c r="D1" s="189"/>
+      <c r="E1" s="189"/>
       <c r="F1" s="38"/>
       <c r="G1" s="61"/>
       <c r="H1" s="35"/>
@@ -9543,32 +9544,32 @@
       <c r="J1" s="62"/>
     </row>
     <row r="2" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="214" t="s">
+      <c r="A2" s="223" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="215"/>
-      <c r="C2" s="210" t="s">
+      <c r="B2" s="224"/>
+      <c r="C2" s="236" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="211"/>
-      <c r="E2" s="212" t="s">
+      <c r="D2" s="237"/>
+      <c r="E2" s="238" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="216"/>
-      <c r="B3" s="217"/>
+      <c r="A3" s="225"/>
+      <c r="B3" s="226"/>
       <c r="C3" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="213"/>
+      <c r="E3" s="239"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="196"/>
-      <c r="B4" s="197"/>
+      <c r="A4" s="206"/>
+      <c r="B4" s="207"/>
       <c r="C4" s="39"/>
       <c r="D4" s="51"/>
       <c r="E4" s="52"/>
@@ -9580,8 +9581,8 @@
       <c r="K4" s="98"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="198"/>
-      <c r="B5" s="199"/>
+      <c r="A5" s="187"/>
+      <c r="B5" s="188"/>
       <c r="C5" s="58"/>
       <c r="D5" s="54"/>
       <c r="E5" s="55"/>
@@ -9593,8 +9594,8 @@
       <c r="K5" s="98"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="198"/>
-      <c r="B6" s="199"/>
+      <c r="A6" s="187"/>
+      <c r="B6" s="188"/>
       <c r="C6" s="39"/>
       <c r="D6" s="51"/>
       <c r="E6" s="52"/>
@@ -9606,8 +9607,8 @@
       <c r="K6" s="98"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="198"/>
-      <c r="B7" s="199"/>
+      <c r="A7" s="187"/>
+      <c r="B7" s="188"/>
       <c r="C7" s="58"/>
       <c r="D7" s="54"/>
       <c r="E7" s="55"/>
@@ -9619,8 +9620,8 @@
       <c r="K7" s="98"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="198"/>
-      <c r="B8" s="199"/>
+      <c r="A8" s="187"/>
+      <c r="B8" s="188"/>
       <c r="C8" s="39"/>
       <c r="D8" s="51"/>
       <c r="E8" s="52"/>
@@ -9632,8 +9633,8 @@
       <c r="K8" s="98"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="198"/>
-      <c r="B9" s="199"/>
+      <c r="A9" s="187"/>
+      <c r="B9" s="188"/>
       <c r="C9" s="58"/>
       <c r="D9" s="54"/>
       <c r="E9" s="55"/>
@@ -9645,8 +9646,8 @@
       <c r="K9" s="98"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="198"/>
-      <c r="B10" s="199"/>
+      <c r="A10" s="187"/>
+      <c r="B10" s="188"/>
       <c r="C10" s="39"/>
       <c r="D10" s="51"/>
       <c r="E10" s="52"/>
@@ -9658,8 +9659,8 @@
       <c r="K10" s="98"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="198"/>
-      <c r="B11" s="199"/>
+      <c r="A11" s="187"/>
+      <c r="B11" s="188"/>
       <c r="C11" s="58"/>
       <c r="D11" s="54"/>
       <c r="E11" s="55"/>
@@ -9671,8 +9672,8 @@
       <c r="K11" s="98"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="198"/>
-      <c r="B12" s="199"/>
+      <c r="A12" s="187"/>
+      <c r="B12" s="188"/>
       <c r="C12" s="39"/>
       <c r="D12" s="51"/>
       <c r="E12" s="52"/>
@@ -9684,8 +9685,8 @@
       <c r="K12" s="98"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="198"/>
-      <c r="B13" s="199"/>
+      <c r="A13" s="187"/>
+      <c r="B13" s="188"/>
       <c r="C13" s="58"/>
       <c r="D13" s="54"/>
       <c r="E13" s="55"/>
@@ -9697,8 +9698,8 @@
       <c r="K13" s="98"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="198"/>
-      <c r="B14" s="199"/>
+      <c r="A14" s="187"/>
+      <c r="B14" s="188"/>
       <c r="C14" s="39"/>
       <c r="D14" s="51"/>
       <c r="E14" s="52"/>
@@ -9710,8 +9711,8 @@
       <c r="K14" s="98"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="198"/>
-      <c r="B15" s="199"/>
+      <c r="A15" s="187"/>
+      <c r="B15" s="188"/>
       <c r="C15" s="58"/>
       <c r="D15" s="54"/>
       <c r="E15" s="55"/>
@@ -9723,8 +9724,8 @@
       <c r="K15" s="98"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="198"/>
-      <c r="B16" s="199"/>
+      <c r="A16" s="187"/>
+      <c r="B16" s="188"/>
       <c r="C16" s="39"/>
       <c r="D16" s="51"/>
       <c r="E16" s="52"/>
@@ -9736,8 +9737,8 @@
       <c r="K16" s="98"/>
     </row>
     <row r="17" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="200"/>
-      <c r="B17" s="201"/>
+      <c r="A17" s="208"/>
+      <c r="B17" s="209"/>
       <c r="C17" s="119"/>
       <c r="D17" s="56"/>
       <c r="E17" s="57"/>
@@ -9749,10 +9750,10 @@
       <c r="K17" s="98"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="227" t="s">
+      <c r="A18" s="221" t="s">
         <v>80</v>
       </c>
-      <c r="B18" s="228"/>
+      <c r="B18" s="222"/>
       <c r="C18" s="120"/>
       <c r="D18" s="120"/>
       <c r="E18" s="121"/>
@@ -9764,23 +9765,23 @@
       <c r="K18" s="98"/>
     </row>
     <row r="19" spans="1:11" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="237" t="s">
+      <c r="A19" s="212" t="s">
         <v>275</v>
       </c>
-      <c r="B19" s="238"/>
-      <c r="C19" s="238"/>
-      <c r="D19" s="238"/>
-      <c r="E19" s="239"/>
+      <c r="B19" s="213"/>
+      <c r="C19" s="213"/>
+      <c r="D19" s="213"/>
+      <c r="E19" s="214"/>
       <c r="F19" s="98"/>
-      <c r="G19" s="236"/>
-      <c r="H19" s="236"/>
-      <c r="I19" s="236"/>
-      <c r="J19" s="236"/>
-      <c r="K19" s="236"/>
+      <c r="G19" s="210"/>
+      <c r="H19" s="210"/>
+      <c r="I19" s="210"/>
+      <c r="J19" s="210"/>
+      <c r="K19" s="210"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="229"/>
-      <c r="B20" s="229"/>
+      <c r="A20" s="211"/>
+      <c r="B20" s="211"/>
       <c r="C20" s="122"/>
       <c r="D20" s="122"/>
       <c r="E20" s="123"/>
@@ -9792,8 +9793,8 @@
       <c r="K20" s="110"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" s="198"/>
-      <c r="B21" s="199"/>
+      <c r="A21" s="187"/>
+      <c r="B21" s="188"/>
       <c r="C21" s="54"/>
       <c r="D21" s="54"/>
       <c r="E21" s="54"/>
@@ -9805,8 +9806,8 @@
       <c r="K21" s="98"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" s="229"/>
-      <c r="B22" s="229"/>
+      <c r="A22" s="211"/>
+      <c r="B22" s="211"/>
       <c r="C22" s="54"/>
       <c r="D22" s="54"/>
       <c r="E22" s="54"/>
@@ -9818,8 +9819,8 @@
       <c r="K22" s="98"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="198"/>
-      <c r="B23" s="199"/>
+      <c r="A23" s="187"/>
+      <c r="B23" s="188"/>
       <c r="C23" s="54"/>
       <c r="D23" s="54"/>
       <c r="E23" s="54"/>
@@ -9831,8 +9832,8 @@
       <c r="K23" s="98"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" s="229"/>
-      <c r="B24" s="229"/>
+      <c r="A24" s="211"/>
+      <c r="B24" s="211"/>
       <c r="C24" s="54"/>
       <c r="D24" s="54"/>
       <c r="E24" s="54"/>
@@ -9844,8 +9845,8 @@
       <c r="K24" s="98"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" s="198"/>
-      <c r="B25" s="199"/>
+      <c r="A25" s="187"/>
+      <c r="B25" s="188"/>
       <c r="C25" s="54"/>
       <c r="D25" s="54"/>
       <c r="E25" s="54"/>
@@ -9857,8 +9858,8 @@
       <c r="K25" s="98"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="229"/>
-      <c r="B26" s="229"/>
+      <c r="A26" s="211"/>
+      <c r="B26" s="211"/>
       <c r="C26" s="54"/>
       <c r="D26" s="54"/>
       <c r="E26" s="54"/>
@@ -9870,8 +9871,8 @@
       <c r="K26" s="98"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" s="198"/>
-      <c r="B27" s="199"/>
+      <c r="A27" s="187"/>
+      <c r="B27" s="188"/>
       <c r="C27" s="54"/>
       <c r="D27" s="54"/>
       <c r="E27" s="54"/>
@@ -9883,8 +9884,8 @@
       <c r="K27" s="98"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A28" s="229"/>
-      <c r="B28" s="229"/>
+      <c r="A28" s="211"/>
+      <c r="B28" s="211"/>
       <c r="C28" s="54"/>
       <c r="D28" s="54"/>
       <c r="E28" s="54"/>
@@ -9896,8 +9897,8 @@
       <c r="K28" s="98"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" s="198"/>
-      <c r="B29" s="199"/>
+      <c r="A29" s="187"/>
+      <c r="B29" s="188"/>
       <c r="C29" s="54"/>
       <c r="D29" s="54"/>
       <c r="E29" s="54"/>
@@ -9909,8 +9910,8 @@
       <c r="K29" s="98"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A30" s="229"/>
-      <c r="B30" s="229"/>
+      <c r="A30" s="211"/>
+      <c r="B30" s="211"/>
       <c r="C30" s="54"/>
       <c r="D30" s="54"/>
       <c r="E30" s="54"/>
@@ -9922,8 +9923,8 @@
       <c r="K30" s="98"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A31" s="198"/>
-      <c r="B31" s="199"/>
+      <c r="A31" s="187"/>
+      <c r="B31" s="188"/>
       <c r="C31" s="54"/>
       <c r="D31" s="54"/>
       <c r="E31" s="54"/>
@@ -9935,8 +9936,8 @@
       <c r="K31" s="98"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A32" s="229"/>
-      <c r="B32" s="229"/>
+      <c r="A32" s="211"/>
+      <c r="B32" s="211"/>
       <c r="C32" s="54"/>
       <c r="D32" s="54"/>
       <c r="E32" s="54"/>
@@ -9948,8 +9949,8 @@
       <c r="K32" s="98"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A33" s="198"/>
-      <c r="B33" s="199"/>
+      <c r="A33" s="187"/>
+      <c r="B33" s="188"/>
       <c r="C33" s="54"/>
       <c r="D33" s="54"/>
       <c r="E33" s="54"/>
@@ -9961,8 +9962,8 @@
       <c r="K33" s="98"/>
     </row>
     <row r="34" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="229"/>
-      <c r="B34" s="229"/>
+      <c r="A34" s="211"/>
+      <c r="B34" s="211"/>
       <c r="C34" s="54"/>
       <c r="D34" s="54"/>
       <c r="E34" s="54"/>
@@ -9974,10 +9975,10 @@
       <c r="K34" s="98"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A35" s="227" t="s">
+      <c r="A35" s="221" t="s">
         <v>80</v>
       </c>
-      <c r="B35" s="228"/>
+      <c r="B35" s="222"/>
       <c r="C35" s="120"/>
       <c r="D35" s="120"/>
       <c r="E35" s="121"/>
@@ -9989,13 +9990,13 @@
       <c r="K35" s="98"/>
     </row>
     <row r="36" spans="1:11" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="226" t="s">
+      <c r="A36" s="235" t="s">
         <v>286</v>
       </c>
-      <c r="B36" s="226"/>
-      <c r="C36" s="226"/>
-      <c r="D36" s="226"/>
-      <c r="E36" s="226"/>
+      <c r="B36" s="235"/>
+      <c r="C36" s="235"/>
+      <c r="D36" s="235"/>
+      <c r="E36" s="235"/>
       <c r="F36" s="98"/>
       <c r="G36" s="99"/>
       <c r="H36" s="98"/>
@@ -10004,15 +10005,15 @@
       <c r="K36" s="98"/>
     </row>
     <row r="37" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="222" t="s">
+      <c r="A37" s="231" t="s">
         <v>79</v>
       </c>
-      <c r="B37" s="223"/>
-      <c r="C37" s="219" t="s">
+      <c r="B37" s="232"/>
+      <c r="C37" s="228" t="s">
         <v>15</v>
       </c>
-      <c r="D37" s="203"/>
-      <c r="E37" s="220" t="s">
+      <c r="D37" s="190"/>
+      <c r="E37" s="229" t="s">
         <v>16</v>
       </c>
       <c r="F37" s="98"/>
@@ -10023,15 +10024,15 @@
       <c r="K37" s="98"/>
     </row>
     <row r="38" spans="1:11" s="6" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="224"/>
-      <c r="B38" s="225"/>
+      <c r="A38" s="233"/>
+      <c r="B38" s="234"/>
       <c r="C38" s="124" t="s">
         <v>4</v>
       </c>
       <c r="D38" s="125" t="s">
         <v>5</v>
       </c>
-      <c r="E38" s="221"/>
+      <c r="E38" s="230"/>
       <c r="F38" s="126"/>
       <c r="G38" s="127"/>
       <c r="H38" s="126"/>
@@ -10040,8 +10041,8 @@
       <c r="K38" s="126"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A39" s="196"/>
-      <c r="B39" s="197"/>
+      <c r="A39" s="206"/>
+      <c r="B39" s="207"/>
       <c r="C39" s="122"/>
       <c r="D39" s="122"/>
       <c r="E39" s="123"/>
@@ -10053,8 +10054,8 @@
       <c r="K39" s="98"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A40" s="198"/>
-      <c r="B40" s="199"/>
+      <c r="A40" s="187"/>
+      <c r="B40" s="188"/>
       <c r="C40" s="54"/>
       <c r="D40" s="54"/>
       <c r="E40" s="128"/>
@@ -10066,8 +10067,8 @@
       <c r="K40" s="98"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A41" s="198"/>
-      <c r="B41" s="199"/>
+      <c r="A41" s="187"/>
+      <c r="B41" s="188"/>
       <c r="C41" s="54"/>
       <c r="D41" s="54"/>
       <c r="E41" s="129"/>
@@ -10079,8 +10080,8 @@
       <c r="K41" s="98"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A42" s="198"/>
-      <c r="B42" s="199"/>
+      <c r="A42" s="187"/>
+      <c r="B42" s="188"/>
       <c r="C42" s="54"/>
       <c r="D42" s="54"/>
       <c r="E42" s="128"/>
@@ -10092,8 +10093,8 @@
       <c r="K42" s="98"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A43" s="198"/>
-      <c r="B43" s="199"/>
+      <c r="A43" s="187"/>
+      <c r="B43" s="188"/>
       <c r="C43" s="54"/>
       <c r="D43" s="54"/>
       <c r="E43" s="129"/>
@@ -10105,8 +10106,8 @@
       <c r="K43" s="98"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A44" s="198"/>
-      <c r="B44" s="199"/>
+      <c r="A44" s="187"/>
+      <c r="B44" s="188"/>
       <c r="C44" s="54"/>
       <c r="D44" s="54"/>
       <c r="E44" s="128"/>
@@ -10118,8 +10119,8 @@
       <c r="K44" s="98"/>
     </row>
     <row r="45" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="200"/>
-      <c r="B45" s="201"/>
+      <c r="A45" s="208"/>
+      <c r="B45" s="209"/>
       <c r="C45" s="54"/>
       <c r="D45" s="54"/>
       <c r="E45" s="129"/>
@@ -10146,13 +10147,13 @@
       <c r="K46" s="98"/>
     </row>
     <row r="47" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="218" t="s">
+      <c r="A47" s="227" t="s">
         <v>284</v>
       </c>
-      <c r="B47" s="218"/>
-      <c r="C47" s="218"/>
-      <c r="D47" s="218"/>
-      <c r="E47" s="218"/>
+      <c r="B47" s="227"/>
+      <c r="C47" s="227"/>
+      <c r="D47" s="227"/>
+      <c r="E47" s="227"/>
       <c r="F47" s="98"/>
       <c r="G47" s="99"/>
       <c r="H47" s="98"/>
@@ -10161,11 +10162,11 @@
       <c r="K47" s="98"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A48" s="196"/>
-      <c r="B48" s="232"/>
-      <c r="C48" s="232"/>
-      <c r="D48" s="232"/>
-      <c r="E48" s="233"/>
+      <c r="A48" s="206"/>
+      <c r="B48" s="219"/>
+      <c r="C48" s="219"/>
+      <c r="D48" s="219"/>
+      <c r="E48" s="220"/>
       <c r="F48" s="98"/>
       <c r="G48" s="99"/>
       <c r="H48" s="98"/>
@@ -10174,11 +10175,11 @@
       <c r="K48" s="98"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A49" s="198"/>
-      <c r="B49" s="230"/>
-      <c r="C49" s="230"/>
-      <c r="D49" s="230"/>
-      <c r="E49" s="231"/>
+      <c r="A49" s="187"/>
+      <c r="B49" s="215"/>
+      <c r="C49" s="215"/>
+      <c r="D49" s="215"/>
+      <c r="E49" s="216"/>
       <c r="F49" s="98"/>
       <c r="G49" s="99"/>
       <c r="H49" s="98"/>
@@ -10187,11 +10188,11 @@
       <c r="K49" s="98"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A50" s="198"/>
-      <c r="B50" s="230"/>
-      <c r="C50" s="230"/>
-      <c r="D50" s="230"/>
-      <c r="E50" s="231"/>
+      <c r="A50" s="187"/>
+      <c r="B50" s="215"/>
+      <c r="C50" s="215"/>
+      <c r="D50" s="215"/>
+      <c r="E50" s="216"/>
       <c r="F50" s="98"/>
       <c r="G50" s="99"/>
       <c r="H50" s="98"/>
@@ -10200,11 +10201,11 @@
       <c r="K50" s="98"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A51" s="198"/>
-      <c r="B51" s="230"/>
-      <c r="C51" s="230"/>
-      <c r="D51" s="230"/>
-      <c r="E51" s="231"/>
+      <c r="A51" s="187"/>
+      <c r="B51" s="215"/>
+      <c r="C51" s="215"/>
+      <c r="D51" s="215"/>
+      <c r="E51" s="216"/>
       <c r="F51" s="98"/>
       <c r="G51" s="99"/>
       <c r="H51" s="98"/>
@@ -10213,11 +10214,11 @@
       <c r="K51" s="98"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A52" s="198"/>
-      <c r="B52" s="230"/>
-      <c r="C52" s="230"/>
-      <c r="D52" s="230"/>
-      <c r="E52" s="231"/>
+      <c r="A52" s="187"/>
+      <c r="B52" s="215"/>
+      <c r="C52" s="215"/>
+      <c r="D52" s="215"/>
+      <c r="E52" s="216"/>
       <c r="F52" s="98"/>
       <c r="G52" s="99"/>
       <c r="H52" s="98"/>
@@ -10226,11 +10227,11 @@
       <c r="K52" s="98"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A53" s="198"/>
-      <c r="B53" s="230"/>
-      <c r="C53" s="230"/>
-      <c r="D53" s="230"/>
-      <c r="E53" s="231"/>
+      <c r="A53" s="187"/>
+      <c r="B53" s="215"/>
+      <c r="C53" s="215"/>
+      <c r="D53" s="215"/>
+      <c r="E53" s="216"/>
       <c r="F53" s="98"/>
       <c r="G53" s="99"/>
       <c r="H53" s="98"/>
@@ -10239,11 +10240,11 @@
       <c r="K53" s="98"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A54" s="198"/>
-      <c r="B54" s="230"/>
-      <c r="C54" s="230"/>
-      <c r="D54" s="230"/>
-      <c r="E54" s="231"/>
+      <c r="A54" s="187"/>
+      <c r="B54" s="215"/>
+      <c r="C54" s="215"/>
+      <c r="D54" s="215"/>
+      <c r="E54" s="216"/>
       <c r="F54" s="98"/>
       <c r="G54" s="99"/>
       <c r="H54" s="98"/>
@@ -10252,11 +10253,11 @@
       <c r="K54" s="98"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A55" s="198"/>
-      <c r="B55" s="230"/>
-      <c r="C55" s="230"/>
-      <c r="D55" s="230"/>
-      <c r="E55" s="231"/>
+      <c r="A55" s="187"/>
+      <c r="B55" s="215"/>
+      <c r="C55" s="215"/>
+      <c r="D55" s="215"/>
+      <c r="E55" s="216"/>
       <c r="F55" s="98"/>
       <c r="G55" s="99"/>
       <c r="H55" s="98"/>
@@ -10265,11 +10266,11 @@
       <c r="K55" s="98"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A56" s="198"/>
-      <c r="B56" s="230"/>
-      <c r="C56" s="230"/>
-      <c r="D56" s="230"/>
-      <c r="E56" s="231"/>
+      <c r="A56" s="187"/>
+      <c r="B56" s="215"/>
+      <c r="C56" s="215"/>
+      <c r="D56" s="215"/>
+      <c r="E56" s="216"/>
       <c r="F56" s="98"/>
       <c r="G56" s="99"/>
       <c r="H56" s="98"/>
@@ -10278,11 +10279,11 @@
       <c r="K56" s="98"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A57" s="198"/>
-      <c r="B57" s="230"/>
-      <c r="C57" s="230"/>
-      <c r="D57" s="230"/>
-      <c r="E57" s="231"/>
+      <c r="A57" s="187"/>
+      <c r="B57" s="215"/>
+      <c r="C57" s="215"/>
+      <c r="D57" s="215"/>
+      <c r="E57" s="216"/>
       <c r="F57" s="98"/>
       <c r="G57" s="99"/>
       <c r="H57" s="98"/>
@@ -10291,11 +10292,11 @@
       <c r="K57" s="98"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A58" s="198"/>
-      <c r="B58" s="230"/>
-      <c r="C58" s="230"/>
-      <c r="D58" s="230"/>
-      <c r="E58" s="231"/>
+      <c r="A58" s="187"/>
+      <c r="B58" s="215"/>
+      <c r="C58" s="215"/>
+      <c r="D58" s="215"/>
+      <c r="E58" s="216"/>
       <c r="F58" s="98"/>
       <c r="G58" s="99"/>
       <c r="H58" s="98"/>
@@ -10304,11 +10305,11 @@
       <c r="K58" s="98"/>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A59" s="198"/>
-      <c r="B59" s="230"/>
-      <c r="C59" s="230"/>
-      <c r="D59" s="230"/>
-      <c r="E59" s="231"/>
+      <c r="A59" s="187"/>
+      <c r="B59" s="215"/>
+      <c r="C59" s="215"/>
+      <c r="D59" s="215"/>
+      <c r="E59" s="216"/>
       <c r="F59" s="98"/>
       <c r="G59" s="99"/>
       <c r="H59" s="98"/>
@@ -10317,11 +10318,11 @@
       <c r="K59" s="98"/>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A60" s="198"/>
-      <c r="B60" s="230"/>
-      <c r="C60" s="230"/>
-      <c r="D60" s="230"/>
-      <c r="E60" s="231"/>
+      <c r="A60" s="187"/>
+      <c r="B60" s="215"/>
+      <c r="C60" s="215"/>
+      <c r="D60" s="215"/>
+      <c r="E60" s="216"/>
       <c r="F60" s="98"/>
       <c r="G60" s="99"/>
       <c r="H60" s="98"/>
@@ -10330,11 +10331,11 @@
       <c r="K60" s="98"/>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A61" s="198"/>
-      <c r="B61" s="230"/>
-      <c r="C61" s="230"/>
-      <c r="D61" s="230"/>
-      <c r="E61" s="231"/>
+      <c r="A61" s="187"/>
+      <c r="B61" s="215"/>
+      <c r="C61" s="215"/>
+      <c r="D61" s="215"/>
+      <c r="E61" s="216"/>
       <c r="F61" s="98"/>
       <c r="G61" s="99"/>
       <c r="H61" s="98"/>
@@ -10343,11 +10344,11 @@
       <c r="K61" s="98"/>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A62" s="198"/>
-      <c r="B62" s="230"/>
-      <c r="C62" s="230"/>
-      <c r="D62" s="230"/>
-      <c r="E62" s="231"/>
+      <c r="A62" s="187"/>
+      <c r="B62" s="215"/>
+      <c r="C62" s="215"/>
+      <c r="D62" s="215"/>
+      <c r="E62" s="216"/>
       <c r="F62" s="98"/>
       <c r="G62" s="99"/>
       <c r="H62" s="98"/>
@@ -10356,11 +10357,11 @@
       <c r="K62" s="98"/>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A63" s="198"/>
-      <c r="B63" s="230"/>
-      <c r="C63" s="230"/>
-      <c r="D63" s="230"/>
-      <c r="E63" s="231"/>
+      <c r="A63" s="187"/>
+      <c r="B63" s="215"/>
+      <c r="C63" s="215"/>
+      <c r="D63" s="215"/>
+      <c r="E63" s="216"/>
       <c r="F63" s="98"/>
       <c r="G63" s="99"/>
       <c r="H63" s="98"/>
@@ -10369,11 +10370,11 @@
       <c r="K63" s="98"/>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A64" s="198"/>
-      <c r="B64" s="230"/>
-      <c r="C64" s="230"/>
-      <c r="D64" s="230"/>
-      <c r="E64" s="231"/>
+      <c r="A64" s="187"/>
+      <c r="B64" s="215"/>
+      <c r="C64" s="215"/>
+      <c r="D64" s="215"/>
+      <c r="E64" s="216"/>
       <c r="F64" s="98"/>
       <c r="G64" s="99"/>
       <c r="H64" s="98"/>
@@ -10382,11 +10383,11 @@
       <c r="K64" s="98"/>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A65" s="198"/>
-      <c r="B65" s="230"/>
-      <c r="C65" s="230"/>
-      <c r="D65" s="230"/>
-      <c r="E65" s="231"/>
+      <c r="A65" s="187"/>
+      <c r="B65" s="215"/>
+      <c r="C65" s="215"/>
+      <c r="D65" s="215"/>
+      <c r="E65" s="216"/>
       <c r="F65" s="98"/>
       <c r="G65" s="99"/>
       <c r="H65" s="98"/>
@@ -10395,11 +10396,11 @@
       <c r="K65" s="98"/>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A66" s="198"/>
-      <c r="B66" s="230"/>
-      <c r="C66" s="230"/>
-      <c r="D66" s="230"/>
-      <c r="E66" s="231"/>
+      <c r="A66" s="187"/>
+      <c r="B66" s="215"/>
+      <c r="C66" s="215"/>
+      <c r="D66" s="215"/>
+      <c r="E66" s="216"/>
       <c r="F66" s="98"/>
       <c r="G66" s="99"/>
       <c r="H66" s="98"/>
@@ -10408,11 +10409,11 @@
       <c r="K66" s="98"/>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A67" s="198"/>
-      <c r="B67" s="230"/>
-      <c r="C67" s="230"/>
-      <c r="D67" s="230"/>
-      <c r="E67" s="231"/>
+      <c r="A67" s="187"/>
+      <c r="B67" s="215"/>
+      <c r="C67" s="215"/>
+      <c r="D67" s="215"/>
+      <c r="E67" s="216"/>
       <c r="F67" s="98"/>
       <c r="G67" s="99"/>
       <c r="H67" s="98"/>
@@ -10421,11 +10422,11 @@
       <c r="K67" s="98"/>
     </row>
     <row r="68" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="200"/>
-      <c r="B68" s="234"/>
-      <c r="C68" s="234"/>
-      <c r="D68" s="234"/>
-      <c r="E68" s="235"/>
+      <c r="A68" s="208"/>
+      <c r="B68" s="217"/>
+      <c r="C68" s="217"/>
+      <c r="D68" s="217"/>
+      <c r="E68" s="218"/>
       <c r="F68" s="98"/>
       <c r="G68" s="99"/>
       <c r="H68" s="98"/>
@@ -10759,6 +10760,61 @@
     <sortCondition ref="A107"/>
   </sortState>
   <mergeCells count="71">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:B3"/>
+    <mergeCell ref="A47:E47"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A36:E36"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A59:E59"/>
+    <mergeCell ref="A48:E48"/>
+    <mergeCell ref="A49:E49"/>
+    <mergeCell ref="A50:E50"/>
+    <mergeCell ref="A51:E51"/>
+    <mergeCell ref="A52:E52"/>
+    <mergeCell ref="A53:E53"/>
+    <mergeCell ref="A54:E54"/>
+    <mergeCell ref="A55:E55"/>
+    <mergeCell ref="A56:E56"/>
+    <mergeCell ref="A57:E57"/>
+    <mergeCell ref="A58:E58"/>
+    <mergeCell ref="A60:E60"/>
+    <mergeCell ref="A61:E61"/>
+    <mergeCell ref="A62:E62"/>
+    <mergeCell ref="A63:E63"/>
+    <mergeCell ref="A68:E68"/>
+    <mergeCell ref="A64:E64"/>
+    <mergeCell ref="A65:E65"/>
+    <mergeCell ref="A66:E66"/>
+    <mergeCell ref="A67:E67"/>
     <mergeCell ref="G19:K19"/>
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="A31:B31"/>
@@ -10775,61 +10831,6 @@
     <mergeCell ref="A19:E19"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A60:E60"/>
-    <mergeCell ref="A61:E61"/>
-    <mergeCell ref="A62:E62"/>
-    <mergeCell ref="A63:E63"/>
-    <mergeCell ref="A68:E68"/>
-    <mergeCell ref="A64:E64"/>
-    <mergeCell ref="A65:E65"/>
-    <mergeCell ref="A66:E66"/>
-    <mergeCell ref="A67:E67"/>
-    <mergeCell ref="A59:E59"/>
-    <mergeCell ref="A48:E48"/>
-    <mergeCell ref="A49:E49"/>
-    <mergeCell ref="A50:E50"/>
-    <mergeCell ref="A51:E51"/>
-    <mergeCell ref="A52:E52"/>
-    <mergeCell ref="A53:E53"/>
-    <mergeCell ref="A54:E54"/>
-    <mergeCell ref="A55:E55"/>
-    <mergeCell ref="A56:E56"/>
-    <mergeCell ref="A57:E57"/>
-    <mergeCell ref="A58:E58"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:B3"/>
-    <mergeCell ref="A47:E47"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A36:E36"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="H1">
@@ -10865,18 +10866,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="240" t="s">
+      <c r="A1" s="265" t="s">
         <v>289</v>
       </c>
-      <c r="B1" s="241"/>
-      <c r="C1" s="241"/>
-      <c r="D1" s="241"/>
+      <c r="B1" s="266"/>
+      <c r="C1" s="266"/>
+      <c r="D1" s="266"/>
     </row>
     <row r="2" spans="1:4" ht="39" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="252" t="s">
+      <c r="A2" s="271" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="253"/>
+      <c r="B2" s="272"/>
       <c r="C2" s="10" t="s">
         <v>21</v>
       </c>
@@ -10885,305 +10886,305 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="254"/>
-      <c r="B3" s="255"/>
+      <c r="A3" s="273"/>
+      <c r="B3" s="274"/>
       <c r="C3" s="12"/>
       <c r="D3" s="13"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="256"/>
-      <c r="B4" s="257"/>
+      <c r="A4" s="275"/>
+      <c r="B4" s="276"/>
       <c r="C4" s="14"/>
       <c r="D4" s="15"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="256"/>
-      <c r="B5" s="257"/>
+      <c r="A5" s="275"/>
+      <c r="B5" s="276"/>
       <c r="C5" s="14"/>
       <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="256"/>
-      <c r="B6" s="257"/>
+      <c r="A6" s="275"/>
+      <c r="B6" s="276"/>
       <c r="C6" s="14"/>
       <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="256"/>
-      <c r="B7" s="257"/>
+      <c r="A7" s="275"/>
+      <c r="B7" s="276"/>
       <c r="C7" s="14"/>
       <c r="D7" s="15"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="256"/>
-      <c r="B8" s="257"/>
+      <c r="A8" s="275"/>
+      <c r="B8" s="276"/>
       <c r="C8" s="14"/>
       <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="269"/>
-      <c r="B9" s="270"/>
+      <c r="A9" s="240"/>
+      <c r="B9" s="244"/>
       <c r="C9" s="16"/>
       <c r="D9" s="17"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="269"/>
-      <c r="B10" s="270"/>
+      <c r="A10" s="240"/>
+      <c r="B10" s="244"/>
       <c r="C10" s="16"/>
       <c r="D10" s="17"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="269"/>
-      <c r="B11" s="270"/>
+      <c r="A11" s="240"/>
+      <c r="B11" s="244"/>
       <c r="C11" s="16"/>
       <c r="D11" s="17"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="269"/>
-      <c r="B12" s="270"/>
+      <c r="A12" s="240"/>
+      <c r="B12" s="244"/>
       <c r="C12" s="16"/>
       <c r="D12" s="17"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="269"/>
-      <c r="B13" s="270"/>
+      <c r="A13" s="240"/>
+      <c r="B13" s="244"/>
       <c r="C13" s="16"/>
       <c r="D13" s="17"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="269"/>
-      <c r="B14" s="270"/>
+      <c r="A14" s="240"/>
+      <c r="B14" s="244"/>
       <c r="C14" s="16"/>
       <c r="D14" s="17"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="269"/>
-      <c r="B15" s="270"/>
+      <c r="A15" s="240"/>
+      <c r="B15" s="244"/>
       <c r="C15" s="16"/>
       <c r="D15" s="17"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="269"/>
-      <c r="B16" s="270"/>
+      <c r="A16" s="240"/>
+      <c r="B16" s="244"/>
       <c r="C16" s="16"/>
       <c r="D16" s="17"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="269"/>
-      <c r="B17" s="270"/>
+      <c r="A17" s="240"/>
+      <c r="B17" s="244"/>
       <c r="C17" s="16"/>
       <c r="D17" s="17"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="269"/>
-      <c r="B18" s="270"/>
+      <c r="A18" s="240"/>
+      <c r="B18" s="244"/>
       <c r="C18" s="16"/>
       <c r="D18" s="17"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="269"/>
-      <c r="B19" s="270"/>
+      <c r="A19" s="240"/>
+      <c r="B19" s="244"/>
       <c r="C19" s="16"/>
       <c r="D19" s="17"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="269"/>
-      <c r="B20" s="270"/>
+      <c r="A20" s="240"/>
+      <c r="B20" s="244"/>
       <c r="C20" s="16"/>
       <c r="D20" s="17"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="269"/>
-      <c r="B21" s="270"/>
+      <c r="A21" s="240"/>
+      <c r="B21" s="244"/>
       <c r="C21" s="16"/>
       <c r="D21" s="17"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="269"/>
-      <c r="B22" s="270"/>
+      <c r="A22" s="240"/>
+      <c r="B22" s="244"/>
       <c r="C22" s="16"/>
       <c r="D22" s="17"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="269"/>
-      <c r="B23" s="270"/>
+      <c r="A23" s="240"/>
+      <c r="B23" s="244"/>
       <c r="C23" s="16"/>
       <c r="D23" s="17"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="269"/>
-      <c r="B24" s="270"/>
+      <c r="A24" s="240"/>
+      <c r="B24" s="244"/>
       <c r="C24" s="16"/>
       <c r="D24" s="17"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="269"/>
-      <c r="B25" s="270"/>
+      <c r="A25" s="240"/>
+      <c r="B25" s="244"/>
       <c r="C25" s="16"/>
       <c r="D25" s="17"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="269"/>
-      <c r="B26" s="270"/>
+      <c r="A26" s="240"/>
+      <c r="B26" s="244"/>
       <c r="C26" s="16"/>
       <c r="D26" s="17"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="269"/>
-      <c r="B27" s="270"/>
+      <c r="A27" s="240"/>
+      <c r="B27" s="244"/>
       <c r="C27" s="16"/>
       <c r="D27" s="17"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="269"/>
-      <c r="B28" s="270"/>
+      <c r="A28" s="240"/>
+      <c r="B28" s="244"/>
       <c r="C28" s="16"/>
       <c r="D28" s="17"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="269"/>
-      <c r="B29" s="270"/>
+      <c r="A29" s="240"/>
+      <c r="B29" s="244"/>
       <c r="C29" s="16"/>
       <c r="D29" s="17"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="269"/>
-      <c r="B30" s="270"/>
+      <c r="A30" s="240"/>
+      <c r="B30" s="244"/>
       <c r="C30" s="16"/>
       <c r="D30" s="17"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="269"/>
-      <c r="B31" s="270"/>
+      <c r="A31" s="240"/>
+      <c r="B31" s="244"/>
       <c r="C31" s="16"/>
       <c r="D31" s="17"/>
     </row>
     <row r="32" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="272"/>
-      <c r="B32" s="273"/>
+      <c r="A32" s="242"/>
+      <c r="B32" s="245"/>
       <c r="C32" s="18"/>
       <c r="D32" s="19"/>
     </row>
     <row r="33" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="244" t="s">
+      <c r="A33" s="269" t="s">
         <v>23</v>
       </c>
-      <c r="B33" s="245"/>
-      <c r="C33" s="245"/>
-      <c r="D33" s="245"/>
+      <c r="B33" s="270"/>
+      <c r="C33" s="270"/>
+      <c r="D33" s="270"/>
     </row>
     <row r="34" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B34" s="242" t="s">
+      <c r="B34" s="267" t="s">
         <v>25</v>
       </c>
-      <c r="C34" s="243"/>
+      <c r="C34" s="268"/>
       <c r="D34" s="21" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="22"/>
-      <c r="B35" s="274"/>
-      <c r="C35" s="275"/>
+      <c r="B35" s="246"/>
+      <c r="C35" s="247"/>
       <c r="D35" s="22"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="23"/>
-      <c r="B36" s="269"/>
-      <c r="C36" s="271"/>
+      <c r="B36" s="240"/>
+      <c r="C36" s="241"/>
       <c r="D36" s="23"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="23"/>
-      <c r="B37" s="269"/>
-      <c r="C37" s="271"/>
+      <c r="B37" s="240"/>
+      <c r="C37" s="241"/>
       <c r="D37" s="23"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="23"/>
-      <c r="B38" s="269"/>
-      <c r="C38" s="271"/>
+      <c r="B38" s="240"/>
+      <c r="C38" s="241"/>
       <c r="D38" s="23"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="23"/>
-      <c r="B39" s="269"/>
-      <c r="C39" s="271"/>
+      <c r="B39" s="240"/>
+      <c r="C39" s="241"/>
       <c r="D39" s="23"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="23"/>
-      <c r="B40" s="269"/>
-      <c r="C40" s="271"/>
+      <c r="B40" s="240"/>
+      <c r="C40" s="241"/>
       <c r="D40" s="23"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="23"/>
-      <c r="B41" s="269"/>
-      <c r="C41" s="271"/>
+      <c r="B41" s="240"/>
+      <c r="C41" s="241"/>
       <c r="D41" s="23"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="23"/>
-      <c r="B42" s="269"/>
-      <c r="C42" s="271"/>
+      <c r="B42" s="240"/>
+      <c r="C42" s="241"/>
       <c r="D42" s="23"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="23"/>
-      <c r="B43" s="269"/>
-      <c r="C43" s="271"/>
+      <c r="B43" s="240"/>
+      <c r="C43" s="241"/>
       <c r="D43" s="23"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="23"/>
-      <c r="B44" s="269"/>
-      <c r="C44" s="271"/>
+      <c r="B44" s="240"/>
+      <c r="C44" s="241"/>
       <c r="D44" s="23"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="23"/>
-      <c r="B45" s="269"/>
-      <c r="C45" s="271"/>
+      <c r="B45" s="240"/>
+      <c r="C45" s="241"/>
       <c r="D45" s="23"/>
     </row>
     <row r="46" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="23"/>
-      <c r="B46" s="272"/>
-      <c r="C46" s="276"/>
+      <c r="B46" s="242"/>
+      <c r="C46" s="243"/>
       <c r="D46" s="24"/>
     </row>
     <row r="47" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="25"/>
-      <c r="B47" s="258" t="s">
+      <c r="B47" s="250" t="s">
         <v>32</v>
       </c>
-      <c r="C47" s="259"/>
-      <c r="D47" s="260"/>
+      <c r="C47" s="251"/>
+      <c r="D47" s="252"/>
       <c r="G47" s="27"/>
       <c r="H47" s="27"/>
       <c r="I47" s="27"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="23"/>
-      <c r="B48" s="246" t="s">
+      <c r="B48" s="253" t="s">
         <v>288</v>
       </c>
-      <c r="C48" s="247"/>
-      <c r="D48" s="248"/>
+      <c r="C48" s="254"/>
+      <c r="D48" s="255"/>
       <c r="G48" s="27"/>
       <c r="H48" s="27"/>
       <c r="I48" s="27"/>
     </row>
     <row r="49" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="23"/>
-      <c r="B49" s="249" t="s">
+      <c r="B49" s="264" t="s">
         <v>33</v>
       </c>
-      <c r="C49" s="247"/>
+      <c r="C49" s="254"/>
       <c r="D49" s="28"/>
       <c r="G49" s="27"/>
       <c r="H49" s="27"/>
@@ -11191,10 +11192,10 @@
     </row>
     <row r="50" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="23"/>
-      <c r="B50" s="249" t="s">
+      <c r="B50" s="264" t="s">
         <v>26</v>
       </c>
-      <c r="C50" s="247"/>
+      <c r="C50" s="254"/>
       <c r="D50" s="29"/>
       <c r="G50" s="27"/>
       <c r="H50" s="27"/>
@@ -11202,82 +11203,82 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="30"/>
-      <c r="B51" s="261" t="s">
+      <c r="B51" s="256" t="s">
         <v>34</v>
       </c>
-      <c r="C51" s="262"/>
-      <c r="D51" s="263"/>
+      <c r="C51" s="257"/>
+      <c r="D51" s="258"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="30"/>
-      <c r="B52" s="264" t="s">
+      <c r="B52" s="259" t="s">
         <v>35</v>
       </c>
-      <c r="C52" s="265"/>
-      <c r="D52" s="266"/>
+      <c r="C52" s="260"/>
+      <c r="D52" s="261"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="30"/>
-      <c r="B53" s="246" t="s">
+      <c r="B53" s="253" t="s">
         <v>288</v>
       </c>
-      <c r="C53" s="247"/>
-      <c r="D53" s="248"/>
+      <c r="C53" s="254"/>
+      <c r="D53" s="255"/>
     </row>
     <row r="54" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="30"/>
-      <c r="B54" s="249" t="s">
+      <c r="B54" s="264" t="s">
         <v>33</v>
       </c>
-      <c r="C54" s="247"/>
+      <c r="C54" s="254"/>
       <c r="D54" s="28"/>
     </row>
     <row r="55" spans="1:9" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="30"/>
-      <c r="B55" s="250" t="s">
+      <c r="B55" s="248" t="s">
         <v>26</v>
       </c>
-      <c r="C55" s="251"/>
+      <c r="C55" s="249"/>
       <c r="D55" s="29"/>
     </row>
     <row r="56" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="23"/>
-      <c r="B56" s="267" t="s">
+      <c r="B56" s="262" t="s">
         <v>36</v>
       </c>
-      <c r="C56" s="262"/>
-      <c r="D56" s="263"/>
+      <c r="C56" s="257"/>
+      <c r="D56" s="258"/>
     </row>
     <row r="57" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="23"/>
-      <c r="B57" s="268" t="s">
+      <c r="B57" s="263" t="s">
         <v>37</v>
       </c>
-      <c r="C57" s="265"/>
-      <c r="D57" s="266"/>
+      <c r="C57" s="260"/>
+      <c r="D57" s="261"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="23"/>
-      <c r="B58" s="246" t="s">
+      <c r="B58" s="253" t="s">
         <v>288</v>
       </c>
-      <c r="C58" s="247"/>
-      <c r="D58" s="248"/>
+      <c r="C58" s="254"/>
+      <c r="D58" s="255"/>
     </row>
     <row r="59" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="23"/>
-      <c r="B59" s="249" t="s">
+      <c r="B59" s="264" t="s">
         <v>33</v>
       </c>
-      <c r="C59" s="247"/>
+      <c r="C59" s="254"/>
       <c r="D59" s="28"/>
     </row>
     <row r="60" spans="1:9" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A60" s="24"/>
-      <c r="B60" s="250" t="s">
+      <c r="B60" s="248" t="s">
         <v>26</v>
       </c>
-      <c r="C60" s="251"/>
+      <c r="C60" s="249"/>
       <c r="D60" s="89"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
@@ -11292,50 +11293,6 @@
     </row>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="B48:D48"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="B52:D52"/>
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="B57:D57"/>
-    <mergeCell ref="B59:C59"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="B34:C34"/>
     <mergeCell ref="A33:D33"/>
@@ -11352,6 +11309,50 @@
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.31" right="0.39370078740157483" top="0.43" bottom="0.19685039370078741" header="0.31496062992125984" footer="0"/>

</xml_diff>